<commit_message>
Schematic and PCB V1 done
</commit_message>
<xml_diff>
--- a/3.Budgeting/BOM.xlsx
+++ b/3.Budgeting/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Mouser No.</t>
   </si>
@@ -216,7 +216,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1x2 conn</t>
+    <t xml:space="preserve">1x2 conn female</t>
   </si>
   <si>
     <t xml:space="preserve">80-C0805F104K1RAUTO
@@ -297,6 +297,35 @@
   </si>
   <si>
     <t xml:space="preserve">1m Shunt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">649-1012938090202ALF
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10129380-902002ALF
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1x2 conn male</t>
   </si>
 </sst>
 </file>
@@ -397,7 +426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -436,18 +465,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -576,7 +593,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -691,7 +708,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>23</v>
@@ -721,7 +738,7 @@
       <c r="C10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -729,13 +746,13 @@
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -743,19 +760,29 @@
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>